<commit_message>
Arreglo de bugs en excepciones Diamante Bruto y Diamante Corte
</commit_message>
<xml_diff>
--- a/.Base_Datos.xlsx
+++ b/.Base_Datos.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -700,6 +700,52 @@
       </c>
       <c r="E12" t="n">
         <v>3116700000</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Santiago Arango</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>12</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>santi@gmail.com</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>7155934</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Bayron Valdés </t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>13</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>bayron2813@gmail.com</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Medellín</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>3015168866</v>
       </c>
     </row>
   </sheetData>
@@ -713,7 +759,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -885,6 +931,123 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>12</v>
+      </c>
+      <c r="B8" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.3 
+El grabado del Diamante es True 
+El origen del diamante es cabello 
+El tamaño del Diamante es 0.5 
+El grabado del Diamante es True 
+El origen del diamante es cenizas 
+El corte del diamante es corazon 
+</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>31/12/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>13</v>
+      </c>
+      <c r="B9" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.8 
+El grabado del Diamante es True 
+El origen del diamante es cenizas 
+El tamaño del Diamante es 0.5 
+El grabado del Diamante es True 
+El origen del diamante es cenizas 
+El corte del diamante es Corazon 
+</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>23/04/2021</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>13</v>
+      </c>
+      <c r="B10" t="n">
+        <v>9</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.6 
+El grabado del Diamante es True 
+El origen del diamante es cenizas 
+El tamaño del Diamante es 0.5 
+El grabado del Diamante es True 
+El origen del diamante es cenizas 
+El corte del diamante es corazon 
+</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>20/04/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" t="n">
+        <v>10</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.5 
+El grabado del Diamante es True 
+El origen del diamante es cenizas 
+</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>20/04/2022</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="n">
+        <v>11</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">El tamaño del Diamante es 0.6 
+El grabado del Diamante es True 
+El origen del diamante es Cabello 
+</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>21/04/2022</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>